<commit_message>
Fixed menu + made ramp in Maya
</commit_message>
<xml_diff>
--- a/Checklist/AGA206 Assessment 2 Checklist.xlsx
+++ b/Checklist/AGA206 Assessment 2 Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmangano1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmangano1\Workspace\Roll-A-Ball\Checklist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FF7A55-E9C5-4B65-BEBB-524E0C1CB6F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4B6CB9E-79C5-46CA-86A2-E9D3C49568AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="2160" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>AGA206 Assessment 2 Checklist</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>Come up with your own</t>
+  </si>
+  <si>
+    <t>Camera shifts down when launched up on jump pad</t>
+  </si>
+  <si>
+    <t>Camera shakes slightly when player is moving fast</t>
+  </si>
+  <si>
+    <t>Made jump pad</t>
+  </si>
+  <si>
+    <t>Changed textures on all walls, changed pickup look, added red lighting</t>
   </si>
 </sst>
 </file>
@@ -474,7 +486,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
@@ -498,11 +510,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,7 +542,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$J$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2753,7 +2765,7 @@
   <dimension ref="B2:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2825,7 +2837,7 @@
       </c>
       <c r="D8" s="8">
         <f>COUNTIFS(J18:J38,TRUE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -2834,7 +2846,7 @@
       </c>
       <c r="D9" s="8">
         <f>K39</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3020,15 +3032,17 @@
       <c r="E20" s="7"/>
       <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G20" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="J20" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
@@ -3260,15 +3274,17 @@
       <c r="E30" s="7"/>
       <c r="F30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G30" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="J30" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.2">
@@ -3380,15 +3396,17 @@
       <c r="E35" s="7"/>
       <c r="F35" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>To Be Done</v>
-      </c>
-      <c r="G35" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>36</v>
+      </c>
       <c r="J35" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
@@ -3404,15 +3422,17 @@
       <c r="E36" s="7"/>
       <c r="F36" s="6" t="str">
         <f t="shared" ref="F36:F38" si="2">IF(J36,"Done","To Be Done")</f>
-        <v>To Be Done</v>
-      </c>
-      <c r="G36" s="17"/>
+        <v>Done</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>37</v>
+      </c>
       <c r="J36" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
@@ -3466,7 +3486,7 @@
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="K39" s="2">
         <f>SUM(K18:K38)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -4053,6 +4073,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="73411d32-3be3-4fb3-bba7-453707a36bfc">
+      <UserInfo>
+        <DisplayName>[Sydney] - ANI/GAM - FEB24 Members</DisplayName>
+        <AccountId>35</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074E599F6BAC38048B1D7AB7C78927E78" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c843b7a1578545a41b78a4f4b27b914d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73411d32-3be3-4fb3-bba7-453707a36bfc" xmlns:ns3="eea594ce-a241-45bb-bb10-367b941c55c8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6d928c0a655351682719421916b6f538" ns2:_="" ns3:_="">
     <xsd:import namespace="73411d32-3be3-4fb3-bba7-453707a36bfc"/>
@@ -4229,30 +4272,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC9BB356-B6ED-4C76-B728-6ABE9F9C7CEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="73411d32-3be3-4fb3-bba7-453707a36bfc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="73411d32-3be3-4fb3-bba7-453707a36bfc">
-      <UserInfo>
-        <DisplayName>[Sydney] - ANI/GAM - FEB24 Members</DisplayName>
-        <AccountId>35</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A2B8EE-6E91-48BB-B190-535F2CAFD38E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D2787F-6F10-461C-83FF-FE2CD5715D14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4269,22 +4307,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A2B8EE-6E91-48BB-B190-535F2CAFD38E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC9BB356-B6ED-4C76-B728-6ABE9F9C7CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="73411d32-3be3-4fb3-bba7-453707a36bfc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>